<commit_message>
cleaned home sales excel
</commit_message>
<xml_diff>
--- a/home_sales.xlsx
+++ b/home_sales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samav\Documents\fanniemae\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61674B0A-7965-42A7-924B-7D50371CDD7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{989D2580-75F7-49AD-BB9A-E7380D9BA54C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{9EEF5B4F-0E4F-41D9-A974-8F46C70F992C}"/>
   </bookViews>
@@ -571,7 +571,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -585,10 +585,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -923,7 +919,7 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="6" t="s">
         <v>146</v>
       </c>
       <c r="C1" s="6" t="s">
@@ -967,8 +963,8 @@
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="10">
-        <f>AVERAGE(C2:N2)</f>
+      <c r="B2">
+        <f t="shared" ref="B2:B33" si="0">AVERAGE(C2:N2)</f>
         <v>44.666666666666664</v>
       </c>
       <c r="C2">
@@ -1012,8 +1008,8 @@
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="10">
-        <f>AVERAGE(C3:N3)</f>
+      <c r="B3">
+        <f t="shared" si="0"/>
         <v>132.5</v>
       </c>
       <c r="C3">
@@ -1057,8 +1053,8 @@
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="10">
-        <f>AVERAGE(C4:N4)</f>
+      <c r="B4">
+        <f t="shared" si="0"/>
         <v>170.41666666666666</v>
       </c>
       <c r="C4">
@@ -1102,8 +1098,8 @@
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="10">
-        <f>AVERAGE(C5:N5)</f>
+      <c r="B5">
+        <f t="shared" si="0"/>
         <v>11.583333333333334</v>
       </c>
       <c r="C5">
@@ -1147,8 +1143,8 @@
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="10">
-        <f>AVERAGE(C6:N6)</f>
+      <c r="B6">
+        <f t="shared" si="0"/>
         <v>10.5</v>
       </c>
       <c r="C6">
@@ -1192,8 +1188,8 @@
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="10">
-        <f>AVERAGE(C7:N7)</f>
+      <c r="B7">
+        <f t="shared" si="0"/>
         <v>25.833333333333332</v>
       </c>
       <c r="C7">
@@ -1237,8 +1233,8 @@
       <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="10">
-        <f>AVERAGE(C8:N8)</f>
+      <c r="B8">
+        <f t="shared" si="0"/>
         <v>13.833333333333334</v>
       </c>
       <c r="C8">
@@ -1282,8 +1278,8 @@
       <c r="A9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="10">
-        <f>AVERAGE(C9:N9)</f>
+      <c r="B9">
+        <f t="shared" si="0"/>
         <v>183.5</v>
       </c>
       <c r="C9">
@@ -1327,8 +1323,8 @@
       <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="10">
-        <f>AVERAGE(C10:N10)</f>
+      <c r="B10">
+        <f t="shared" si="0"/>
         <v>57.333333333333336</v>
       </c>
       <c r="C10">
@@ -1372,8 +1368,8 @@
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="10">
-        <f>AVERAGE(C11:N11)</f>
+      <c r="B11">
+        <f t="shared" si="0"/>
         <v>2.9166666666666665</v>
       </c>
       <c r="C11">
@@ -1417,8 +1413,8 @@
       <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="10">
-        <f>AVERAGE(C12:N12)</f>
+      <c r="B12">
+        <f t="shared" si="0"/>
         <v>88.166666666666671</v>
       </c>
       <c r="C12" s="1">
@@ -1462,8 +1458,8 @@
       <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="10">
-        <f>AVERAGE(C13:N13)</f>
+      <c r="B13">
+        <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
       <c r="C13">
@@ -1507,8 +1503,8 @@
       <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="10">
-        <f>AVERAGE(C14:N14)</f>
+      <c r="B14">
+        <f t="shared" si="0"/>
         <v>29.416666666666668</v>
       </c>
       <c r="C14">
@@ -1552,8 +1548,8 @@
       <c r="A15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="10">
-        <f>AVERAGE(C15:N15)</f>
+      <c r="B15">
+        <f t="shared" si="0"/>
         <v>4.75</v>
       </c>
       <c r="C15">
@@ -1597,8 +1593,8 @@
       <c r="A16" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="10">
-        <f>AVERAGE(C16:N16)</f>
+      <c r="B16">
+        <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
       <c r="C16">
@@ -1642,8 +1638,8 @@
       <c r="A17" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="10">
-        <f>AVERAGE(C17:N17)</f>
+      <c r="B17">
+        <f t="shared" si="0"/>
         <v>3.0833333333333335</v>
       </c>
       <c r="C17">
@@ -1687,8 +1683,8 @@
       <c r="A18" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="10">
-        <f>AVERAGE(C18:N18)</f>
+      <c r="B18">
+        <f t="shared" si="0"/>
         <v>11.666666666666666</v>
       </c>
       <c r="C18">
@@ -1732,8 +1728,8 @@
       <c r="A19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="10">
-        <f>AVERAGE(C19:N19)</f>
+      <c r="B19">
+        <f t="shared" si="0"/>
         <v>5.583333333333333</v>
       </c>
       <c r="C19">
@@ -1777,8 +1773,8 @@
       <c r="A20" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="10">
-        <f>AVERAGE(C20:N20)</f>
+      <c r="B20">
+        <f t="shared" si="0"/>
         <v>51.75</v>
       </c>
       <c r="C20">
@@ -1822,8 +1818,8 @@
       <c r="A21" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="10">
-        <f>AVERAGE(C21:N21)</f>
+      <c r="B21">
+        <f t="shared" si="0"/>
         <v>43.25</v>
       </c>
       <c r="C21">
@@ -1867,8 +1863,8 @@
       <c r="A22" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="10">
-        <f>AVERAGE(C22:N22)</f>
+      <c r="B22">
+        <f t="shared" si="0"/>
         <v>27.5</v>
       </c>
       <c r="C22">
@@ -1912,8 +1908,8 @@
       <c r="A23" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="10">
-        <f>AVERAGE(C23:N23)</f>
+      <c r="B23">
+        <f t="shared" si="0"/>
         <v>2.6666666666666665</v>
       </c>
       <c r="C23">
@@ -1957,8 +1953,8 @@
       <c r="A24" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="10">
-        <f>AVERAGE(C24:N24)</f>
+      <c r="B24">
+        <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
       <c r="C24">
@@ -2002,8 +1998,8 @@
       <c r="A25" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="10">
-        <f>AVERAGE(C25:N25)</f>
+      <c r="B25">
+        <f t="shared" si="0"/>
         <v>32.666666666666664</v>
       </c>
       <c r="C25">
@@ -2047,8 +2043,8 @@
       <c r="A26" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="10">
-        <f>AVERAGE(C26:N26)</f>
+      <c r="B26">
+        <f t="shared" si="0"/>
         <v>295.33333333333331</v>
       </c>
       <c r="C26">
@@ -2092,8 +2088,8 @@
       <c r="A27" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="10">
-        <f>AVERAGE(C27:N27)</f>
+      <c r="B27">
+        <f t="shared" si="0"/>
         <v>411.66666666666669</v>
       </c>
       <c r="C27">
@@ -2137,8 +2133,8 @@
       <c r="A28" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="10">
-        <f>AVERAGE(C28:N28)</f>
+      <c r="B28">
+        <f t="shared" si="0"/>
         <v>14.75</v>
       </c>
       <c r="C28">
@@ -2182,8 +2178,8 @@
       <c r="A29" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="10">
-        <f>AVERAGE(C29:N29)</f>
+      <c r="B29">
+        <f t="shared" si="0"/>
         <v>19.833333333333332</v>
       </c>
       <c r="C29">
@@ -2227,8 +2223,8 @@
       <c r="A30" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="10">
-        <f>AVERAGE(C30:N30)</f>
+      <c r="B30">
+        <f t="shared" si="0"/>
         <v>4.666666666666667</v>
       </c>
       <c r="C30">
@@ -2272,8 +2268,8 @@
       <c r="A31" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="10">
-        <f>AVERAGE(C31:N31)</f>
+      <c r="B31">
+        <f t="shared" si="0"/>
         <v>3.6666666666666665</v>
       </c>
       <c r="C31">
@@ -2317,8 +2313,8 @@
       <c r="A32" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="10">
-        <f>AVERAGE(C32:N32)</f>
+      <c r="B32">
+        <f t="shared" si="0"/>
         <v>45.583333333333336</v>
       </c>
       <c r="C32">
@@ -2362,8 +2358,8 @@
       <c r="A33" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="10">
-        <f>AVERAGE(C33:N33)</f>
+      <c r="B33">
+        <f t="shared" si="0"/>
         <v>10.666666666666666</v>
       </c>
       <c r="C33">
@@ -2407,8 +2403,8 @@
       <c r="A34" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B34" s="10">
-        <f>AVERAGE(C34:N34)</f>
+      <c r="B34">
+        <f t="shared" ref="B34:B65" si="1">AVERAGE(C34:N34)</f>
         <v>43.833333333333336</v>
       </c>
       <c r="C34">
@@ -2452,8 +2448,8 @@
       <c r="A35" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B35" s="10">
-        <f>AVERAGE(C35:N35)</f>
+      <c r="B35">
+        <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="C35">
@@ -2497,8 +2493,8 @@
       <c r="A36" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B36" s="10">
-        <f>AVERAGE(C36:N36)</f>
+      <c r="B36">
+        <f t="shared" si="1"/>
         <v>25.416666666666668</v>
       </c>
       <c r="C36">
@@ -2542,8 +2538,8 @@
       <c r="A37" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B37" s="10">
-        <f>AVERAGE(C37:N37)</f>
+      <c r="B37">
+        <f t="shared" si="1"/>
         <v>1.25</v>
       </c>
       <c r="C37">
@@ -2587,8 +2583,8 @@
       <c r="A38" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="10">
-        <f>AVERAGE(C38:N38)</f>
+      <c r="B38">
+        <f t="shared" si="1"/>
         <v>11.666666666666666</v>
       </c>
       <c r="C38">
@@ -2632,8 +2628,8 @@
       <c r="A39" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B39" s="10">
-        <f>AVERAGE(C39:N39)</f>
+      <c r="B39">
+        <f t="shared" si="1"/>
         <v>23.833333333333332</v>
       </c>
       <c r="C39">
@@ -2677,8 +2673,8 @@
       <c r="A40" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B40" s="10">
-        <f>AVERAGE(C40:N40)</f>
+      <c r="B40">
+        <f t="shared" si="1"/>
         <v>922.75</v>
       </c>
       <c r="C40">
@@ -2722,8 +2718,8 @@
       <c r="A41" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B41" s="10">
-        <f>AVERAGE(C41:N41)</f>
+      <c r="B41">
+        <f t="shared" si="1"/>
         <v>11.75</v>
       </c>
       <c r="C41">
@@ -2767,8 +2763,8 @@
       <c r="A42" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B42" s="10">
-        <f>AVERAGE(C42:N42)</f>
+      <c r="B42">
+        <f t="shared" si="1"/>
         <v>71.083333333333329</v>
       </c>
       <c r="C42">
@@ -2812,8 +2808,8 @@
       <c r="A43" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B43" s="10">
-        <f>AVERAGE(C43:N43)</f>
+      <c r="B43">
+        <f t="shared" si="1"/>
         <v>13.25</v>
       </c>
       <c r="C43">
@@ -2857,8 +2853,8 @@
       <c r="A44" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B44" s="10">
-        <f>AVERAGE(C44:N44)</f>
+      <c r="B44">
+        <f t="shared" si="1"/>
         <v>34.916666666666664</v>
       </c>
       <c r="C44">
@@ -2902,8 +2898,8 @@
       <c r="A45" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B45" s="10">
-        <f>AVERAGE(C45:N45)</f>
+      <c r="B45">
+        <f t="shared" si="1"/>
         <v>10.666666666666666</v>
       </c>
       <c r="C45">
@@ -2947,8 +2943,8 @@
       <c r="A46" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B46" s="10">
-        <f>AVERAGE(C46:N46)</f>
+      <c r="B46">
+        <f t="shared" si="1"/>
         <v>45.583333333333336</v>
       </c>
       <c r="C46">
@@ -2992,8 +2988,8 @@
       <c r="A47" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B47" s="10">
-        <f>AVERAGE(C47:N47)</f>
+      <c r="B47">
+        <f t="shared" si="1"/>
         <v>107.5</v>
       </c>
       <c r="C47">
@@ -3037,8 +3033,8 @@
       <c r="A48" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B48" s="10">
-        <f>AVERAGE(C48:N48)</f>
+      <c r="B48">
+        <f t="shared" si="1"/>
         <v>22.75</v>
       </c>
       <c r="C48">
@@ -3082,8 +3078,8 @@
       <c r="A49" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B49" s="10">
-        <f>AVERAGE(C49:N49)</f>
+      <c r="B49">
+        <f t="shared" si="1"/>
         <v>8.8333333333333339</v>
       </c>
       <c r="C49">
@@ -3127,8 +3123,8 @@
       <c r="A50" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B50" s="10">
-        <f>AVERAGE(C50:N50)</f>
+      <c r="B50">
+        <f t="shared" si="1"/>
         <v>11.333333333333334</v>
       </c>
       <c r="C50">
@@ -3172,8 +3168,8 @@
       <c r="A51" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B51" s="10">
-        <f>AVERAGE(C51:N51)</f>
+      <c r="B51">
+        <f t="shared" si="1"/>
         <v>40.416666666666664</v>
       </c>
       <c r="C51">
@@ -3217,8 +3213,8 @@
       <c r="A52" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B52" s="10">
-        <f>AVERAGE(C52:N52)</f>
+      <c r="B52">
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="C52">
@@ -3262,8 +3258,8 @@
       <c r="A53" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B53" s="10">
-        <f>AVERAGE(C53:N53)</f>
+      <c r="B53">
+        <f t="shared" si="1"/>
         <v>9.3333333333333339</v>
       </c>
       <c r="C53">
@@ -3307,8 +3303,8 @@
       <c r="A54" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B54" s="10">
-        <f>AVERAGE(C54:N54)</f>
+      <c r="B54">
+        <f t="shared" si="1"/>
         <v>18.083333333333332</v>
       </c>
       <c r="C54">
@@ -3352,8 +3348,8 @@
       <c r="A55" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="10">
-        <f>AVERAGE(C55:N55)</f>
+      <c r="B55">
+        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
       <c r="C55">
@@ -3397,8 +3393,8 @@
       <c r="A56" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="10">
-        <f>AVERAGE(C56:N56)</f>
+      <c r="B56">
+        <f t="shared" si="1"/>
         <v>17.666666666666668</v>
       </c>
       <c r="C56">
@@ -3442,8 +3438,8 @@
       <c r="A57" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B57" s="10">
-        <f>AVERAGE(C57:N57)</f>
+      <c r="B57">
+        <f t="shared" si="1"/>
         <v>161.66666666666666</v>
       </c>
       <c r="C57">
@@ -3487,8 +3483,8 @@
       <c r="A58" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B58" s="10">
-        <f>AVERAGE(C58:N58)</f>
+      <c r="B58">
+        <f t="shared" si="1"/>
         <v>108.08333333333333</v>
       </c>
       <c r="C58">
@@ -3532,8 +3528,8 @@
       <c r="A59" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B59" s="10">
-        <f>AVERAGE(C59:N59)</f>
+      <c r="B59">
+        <f t="shared" si="1"/>
         <v>24.166666666666668</v>
       </c>
       <c r="C59">
@@ -3577,8 +3573,8 @@
       <c r="A60" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B60" s="10">
-        <f>AVERAGE(C60:N60)</f>
+      <c r="B60">
+        <f t="shared" si="1"/>
         <v>325.08333333333331</v>
       </c>
       <c r="C60">
@@ -3622,8 +3618,8 @@
       <c r="A61" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B61" s="10">
-        <f>AVERAGE(C61:N61)</f>
+      <c r="B61">
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="C61">
@@ -3667,8 +3663,8 @@
       <c r="A62" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B62" s="10">
-        <f>AVERAGE(C62:N62)</f>
+      <c r="B62">
+        <f t="shared" si="1"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="C62">
@@ -3712,8 +3708,8 @@
       <c r="A63" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B63" s="10">
-        <f>AVERAGE(C63:N63)</f>
+      <c r="B63">
+        <f t="shared" si="1"/>
         <v>27.333333333333332</v>
       </c>
       <c r="C63">
@@ -3757,8 +3753,8 @@
       <c r="A64" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B64" s="10">
-        <f>AVERAGE(C64:N64)</f>
+      <c r="B64">
+        <f t="shared" si="1"/>
         <v>51.5</v>
       </c>
       <c r="C64">
@@ -3802,8 +3798,8 @@
       <c r="A65" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B65" s="10">
-        <f>AVERAGE(C65:N65)</f>
+      <c r="B65">
+        <f t="shared" si="1"/>
         <v>122.33333333333333</v>
       </c>
       <c r="C65">
@@ -3847,8 +3843,8 @@
       <c r="A66" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B66" s="10">
-        <f>AVERAGE(C66:N66)</f>
+      <c r="B66">
+        <f t="shared" ref="B66:B97" si="2">AVERAGE(C66:N66)</f>
         <v>4.75</v>
       </c>
       <c r="C66">
@@ -3892,8 +3888,8 @@
       <c r="A67" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B67" s="10">
-        <f>AVERAGE(C67:N67)</f>
+      <c r="B67">
+        <f t="shared" si="2"/>
         <v>28.666666666666668</v>
       </c>
       <c r="C67">
@@ -3937,8 +3933,8 @@
       <c r="A68" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B68" s="10">
-        <f>AVERAGE(C68:N68)</f>
+      <c r="B68">
+        <f t="shared" si="2"/>
         <v>18.083333333333332</v>
       </c>
       <c r="C68">
@@ -3982,8 +3978,8 @@
       <c r="A69" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B69" s="10">
-        <f>AVERAGE(C69:N69)</f>
+      <c r="B69">
+        <f t="shared" si="2"/>
         <v>18.333333333333332</v>
       </c>
       <c r="C69">
@@ -4027,8 +4023,8 @@
       <c r="A70" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B70" s="10">
-        <f>AVERAGE(C70:N70)</f>
+      <c r="B70">
+        <f t="shared" si="2"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="C70">
@@ -4072,8 +4068,8 @@
       <c r="A71" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B71" s="10">
-        <f>AVERAGE(C71:N71)</f>
+      <c r="B71">
+        <f t="shared" si="2"/>
         <v>8.5833333333333339</v>
       </c>
       <c r="C71">
@@ -4117,8 +4113,8 @@
       <c r="A72" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B72" s="10">
-        <f>AVERAGE(C72:N72)</f>
+      <c r="B72">
+        <f t="shared" si="2"/>
         <v>377.41666666666669</v>
       </c>
       <c r="C72">
@@ -4162,8 +4158,8 @@
       <c r="A73" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B73" s="10">
-        <f>AVERAGE(C73:N73)</f>
+      <c r="B73">
+        <f t="shared" si="2"/>
         <v>59.5</v>
       </c>
       <c r="C73">
@@ -4207,8 +4203,8 @@
       <c r="A74" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B74" s="10">
-        <f>AVERAGE(C74:N74)</f>
+      <c r="B74">
+        <f t="shared" si="2"/>
         <v>8.4166666666666661</v>
       </c>
       <c r="C74">
@@ -4252,8 +4248,8 @@
       <c r="A75" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B75" s="10">
-        <f>AVERAGE(C75:N75)</f>
+      <c r="B75">
+        <f t="shared" si="2"/>
         <v>88.083333333333329</v>
       </c>
       <c r="C75">
@@ -4297,8 +4293,8 @@
       <c r="A76" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B76" s="10">
-        <f>AVERAGE(C76:N76)</f>
+      <c r="B76">
+        <f t="shared" si="2"/>
         <v>10.416666666666666</v>
       </c>
       <c r="C76">
@@ -4342,8 +4338,8 @@
       <c r="A77" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B77" s="10">
-        <f>AVERAGE(C77:N77)</f>
+      <c r="B77">
+        <f t="shared" si="2"/>
         <v>39.75</v>
       </c>
       <c r="C77">
@@ -4387,8 +4383,8 @@
       <c r="A78" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B78" s="10">
-        <f>AVERAGE(C78:N78)</f>
+      <c r="B78">
+        <f t="shared" si="2"/>
         <v>13.583333333333334</v>
       </c>
       <c r="C78">
@@ -4432,8 +4428,8 @@
       <c r="A79" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B79" s="10">
-        <f>AVERAGE(C79:N79)</f>
+      <c r="B79">
+        <f t="shared" si="2"/>
         <v>13.583333333333334</v>
       </c>
       <c r="C79">
@@ -4477,8 +4473,8 @@
       <c r="A80" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B80" s="10">
-        <f>AVERAGE(C80:N80)</f>
+      <c r="B80">
+        <f t="shared" si="2"/>
         <v>12.25</v>
       </c>
       <c r="C80">
@@ -4522,8 +4518,8 @@
       <c r="A81" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B81" s="10">
-        <f>AVERAGE(C81:N81)</f>
+      <c r="B81">
+        <f t="shared" si="2"/>
         <v>15.5</v>
       </c>
       <c r="C81">
@@ -4567,8 +4563,8 @@
       <c r="A82" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B82" s="10">
-        <f>AVERAGE(C82:N82)</f>
+      <c r="B82">
+        <f t="shared" si="2"/>
         <v>14.333333333333334</v>
       </c>
       <c r="C82">
@@ -4612,8 +4608,8 @@
       <c r="A83" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B83" s="10">
-        <f>AVERAGE(C83:N83)</f>
+      <c r="B83">
+        <f t="shared" si="2"/>
         <v>71.083333333333329</v>
       </c>
       <c r="C83">
@@ -4657,8 +4653,8 @@
       <c r="A84" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B84" s="10">
-        <f>AVERAGE(C84:N84)</f>
+      <c r="B84">
+        <f t="shared" si="2"/>
         <v>25.083333333333332</v>
       </c>
       <c r="C84">
@@ -4702,8 +4698,8 @@
       <c r="A85" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B85" s="10">
-        <f>AVERAGE(C85:N85)</f>
+      <c r="B85">
+        <f t="shared" si="2"/>
         <v>46.5</v>
       </c>
       <c r="C85">
@@ -4747,8 +4743,8 @@
       <c r="A86" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B86" s="10">
-        <f>AVERAGE(C86:N86)</f>
+      <c r="B86">
+        <f t="shared" si="2"/>
         <v>183.25</v>
       </c>
       <c r="C86">
@@ -4792,8 +4788,8 @@
       <c r="A87" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B87" s="10">
-        <f>AVERAGE(C87:N87)</f>
+      <c r="B87">
+        <f t="shared" si="2"/>
         <v>246.08333333333334</v>
       </c>
       <c r="C87">
@@ -4837,8 +4833,8 @@
       <c r="A88" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B88" s="10">
-        <f>AVERAGE(C88:N88)</f>
+      <c r="B88">
+        <f t="shared" si="2"/>
         <v>17.583333333333332</v>
       </c>
       <c r="C88">
@@ -4882,8 +4878,8 @@
       <c r="A89" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B89" s="10">
-        <f>AVERAGE(C89:N89)</f>
+      <c r="B89">
+        <f t="shared" si="2"/>
         <v>20.25</v>
       </c>
       <c r="C89">
@@ -4927,8 +4923,8 @@
       <c r="A90" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B90" s="10">
-        <f>AVERAGE(C90:N90)</f>
+      <c r="B90">
+        <f t="shared" si="2"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="C90">
@@ -4972,8 +4968,8 @@
       <c r="A91" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B91" s="10">
-        <f>AVERAGE(C91:N91)</f>
+      <c r="B91">
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="C91">
@@ -5017,8 +5013,8 @@
       <c r="A92" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B92" s="10">
-        <f>AVERAGE(C92:N92)</f>
+      <c r="B92">
+        <f t="shared" si="2"/>
         <v>51.416666666666664</v>
       </c>
       <c r="C92">
@@ -5062,8 +5058,8 @@
       <c r="A93" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B93" s="10">
-        <f>AVERAGE(C93:N93)</f>
+      <c r="B93">
+        <f t="shared" si="2"/>
         <v>23.5</v>
       </c>
       <c r="C93">
@@ -5107,8 +5103,8 @@
       <c r="A94" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B94" s="10">
-        <f>AVERAGE(C94:N94)</f>
+      <c r="B94">
+        <f t="shared" si="2"/>
         <v>12.833333333333334</v>
       </c>
       <c r="C94">
@@ -5152,8 +5148,8 @@
       <c r="A95" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B95" s="10">
-        <f>AVERAGE(C95:N95)</f>
+      <c r="B95">
+        <f t="shared" si="2"/>
         <v>40.916666666666664</v>
       </c>
       <c r="C95">
@@ -5197,8 +5193,8 @@
       <c r="A96" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B96" s="10">
-        <f>AVERAGE(C96:N96)</f>
+      <c r="B96">
+        <f t="shared" si="2"/>
         <v>22.416666666666668</v>
       </c>
       <c r="C96">
@@ -5242,8 +5238,8 @@
       <c r="A97" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B97" s="10">
-        <f>AVERAGE(C97:N97)</f>
+      <c r="B97">
+        <f t="shared" si="2"/>
         <v>18.75</v>
       </c>
       <c r="C97">
@@ -5287,8 +5283,8 @@
       <c r="A98" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B98" s="10">
-        <f>AVERAGE(C98:N98)</f>
+      <c r="B98">
+        <f t="shared" ref="B98:B129" si="3">AVERAGE(C98:N98)</f>
         <v>138.33333333333334</v>
       </c>
       <c r="C98">
@@ -5332,8 +5328,8 @@
       <c r="A99" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B99" s="10">
-        <f>AVERAGE(C99:N99)</f>
+      <c r="B99">
+        <f t="shared" si="3"/>
         <v>27.416666666666668</v>
       </c>
       <c r="C99">
@@ -5377,8 +5373,8 @@
       <c r="A100" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B100" s="10">
-        <f>AVERAGE(C100:N100)</f>
+      <c r="B100">
+        <f t="shared" si="3"/>
         <v>14.5</v>
       </c>
       <c r="C100">
@@ -5422,8 +5418,8 @@
       <c r="A101" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B101" s="10">
-        <f>AVERAGE(C101:N101)</f>
+      <c r="B101">
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="C101">
@@ -5467,8 +5463,8 @@
       <c r="A102" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B102" s="10">
-        <f>AVERAGE(C102:N102)</f>
+      <c r="B102">
+        <f t="shared" si="3"/>
         <v>423.08333333333331</v>
       </c>
       <c r="C102">
@@ -5512,8 +5508,8 @@
       <c r="A103" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B103" s="10">
-        <f>AVERAGE(C103:N103)</f>
+      <c r="B103">
+        <f t="shared" si="3"/>
         <v>30.583333333333332</v>
       </c>
       <c r="C103">
@@ -5557,8 +5553,8 @@
       <c r="A104" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B104" s="10">
-        <f>AVERAGE(C104:N104)</f>
+      <c r="B104">
+        <f t="shared" si="3"/>
         <v>12.25</v>
       </c>
       <c r="C104">
@@ -5602,8 +5598,8 @@
       <c r="A105" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B105" s="10">
-        <f>AVERAGE(C105:N105)</f>
+      <c r="B105">
+        <f t="shared" si="3"/>
         <v>6.583333333333333</v>
       </c>
       <c r="C105">
@@ -5647,8 +5643,8 @@
       <c r="A106" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B106" s="10">
-        <f>AVERAGE(C106:N106)</f>
+      <c r="B106">
+        <f t="shared" si="3"/>
         <v>209.08333333333334</v>
       </c>
       <c r="C106">
@@ -5692,8 +5688,8 @@
       <c r="A107" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B107" s="10">
-        <f>AVERAGE(C107:N107)</f>
+      <c r="B107">
+        <f t="shared" si="3"/>
         <v>3.75</v>
       </c>
       <c r="C107">
@@ -5737,8 +5733,8 @@
       <c r="A108" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B108" s="10">
-        <f>AVERAGE(C108:N108)</f>
+      <c r="B108">
+        <f t="shared" si="3"/>
         <v>91.5</v>
       </c>
       <c r="C108">
@@ -5782,8 +5778,8 @@
       <c r="A109" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B109" s="10">
-        <f>AVERAGE(C109:N109)</f>
+      <c r="B109">
+        <f t="shared" si="3"/>
         <v>94</v>
       </c>
       <c r="C109">
@@ -5827,8 +5823,8 @@
       <c r="A110" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B110" s="10">
-        <f>AVERAGE(C110:N110)</f>
+      <c r="B110">
+        <f t="shared" si="3"/>
         <v>18.166666666666668</v>
       </c>
       <c r="C110">
@@ -5872,8 +5868,8 @@
       <c r="A111" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B111" s="10">
-        <f>AVERAGE(C111:N111)</f>
+      <c r="B111">
+        <f t="shared" si="3"/>
         <v>65.666666666666671</v>
       </c>
       <c r="C111">
@@ -5917,8 +5913,8 @@
       <c r="A112" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B112" s="10">
-        <f>AVERAGE(C112:N112)</f>
+      <c r="B112">
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="C112">
@@ -5962,8 +5958,8 @@
       <c r="A113" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B113" s="10">
-        <f>AVERAGE(C113:N113)</f>
+      <c r="B113">
+        <f t="shared" si="3"/>
         <v>21.5</v>
       </c>
       <c r="C113">
@@ -6007,8 +6003,8 @@
       <c r="A114" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B114" s="10">
-        <f>AVERAGE(C114:N114)</f>
+      <c r="B114">
+        <f t="shared" si="3"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="C114">
@@ -6052,8 +6048,8 @@
       <c r="A115" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B115" s="10">
-        <f>AVERAGE(C115:N115)</f>
+      <c r="B115">
+        <f t="shared" si="3"/>
         <v>50.416666666666664</v>
       </c>
       <c r="C115">
@@ -6097,8 +6093,8 @@
       <c r="A116" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B116" s="10">
-        <f>AVERAGE(C116:N116)</f>
+      <c r="B116">
+        <f t="shared" si="3"/>
         <v>19.666666666666668</v>
       </c>
       <c r="C116">
@@ -6142,8 +6138,8 @@
       <c r="A117" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B117" s="10">
-        <f>AVERAGE(C117:N117)</f>
+      <c r="B117">
+        <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
       <c r="C117">
@@ -6187,8 +6183,8 @@
       <c r="A118" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B118" s="10">
-        <f>AVERAGE(C118:N118)</f>
+      <c r="B118">
+        <f t="shared" si="3"/>
         <v>144.16666666666666</v>
       </c>
       <c r="C118">
@@ -6232,8 +6228,8 @@
       <c r="A119" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B119" s="10">
-        <f>AVERAGE(C119:N119)</f>
+      <c r="B119">
+        <f t="shared" si="3"/>
         <v>166.83333333333334</v>
       </c>
       <c r="C119">
@@ -6277,8 +6273,8 @@
       <c r="A120" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B120" s="10">
-        <f>AVERAGE(C120:N120)</f>
+      <c r="B120">
+        <f t="shared" si="3"/>
         <v>31.333333333333332</v>
       </c>
       <c r="C120">
@@ -6322,8 +6318,8 @@
       <c r="A121" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B121" s="10">
-        <f>AVERAGE(C121:N121)</f>
+      <c r="B121">
+        <f t="shared" si="3"/>
         <v>153.08333333333334</v>
       </c>
       <c r="C121">
@@ -6367,8 +6363,8 @@
       <c r="A122" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B122" s="10">
-        <f>AVERAGE(C122:N122)</f>
+      <c r="B122">
+        <f t="shared" si="3"/>
         <v>3.5</v>
       </c>
       <c r="C122">
@@ -6412,8 +6408,8 @@
       <c r="A123" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B123" s="10">
-        <f>AVERAGE(C123:N123)</f>
+      <c r="B123">
+        <f t="shared" si="3"/>
         <v>7.833333333333333</v>
       </c>
       <c r="C123">
@@ -6457,8 +6453,8 @@
       <c r="A124" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B124" s="10">
-        <f>AVERAGE(C124:N124)</f>
+      <c r="B124">
+        <f t="shared" si="3"/>
         <v>17.333333333333332</v>
       </c>
       <c r="C124">
@@ -6502,8 +6498,8 @@
       <c r="A125" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B125" s="10">
-        <f>AVERAGE(C125:N125)</f>
+      <c r="B125">
+        <f t="shared" si="3"/>
         <v>473.83333333333331</v>
       </c>
       <c r="C125">
@@ -6547,8 +6543,8 @@
       <c r="A126" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B126" s="10">
-        <f>AVERAGE(C126:N126)</f>
+      <c r="B126">
+        <f t="shared" si="3"/>
         <v>45.5</v>
       </c>
       <c r="C126">
@@ -6592,8 +6588,8 @@
       <c r="A127" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B127" s="10">
-        <f>AVERAGE(C127:N127)</f>
+      <c r="B127">
+        <f t="shared" si="3"/>
         <v>25.083333333333332</v>
       </c>
       <c r="C127">
@@ -6637,8 +6633,8 @@
       <c r="A128" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B128" s="10">
-        <f>AVERAGE(C128:N128)</f>
+      <c r="B128">
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="C128">
@@ -6682,8 +6678,8 @@
       <c r="A129" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B129" s="10">
-        <f>AVERAGE(C129:N129)</f>
+      <c r="B129">
+        <f t="shared" si="3"/>
         <v>35.166666666666664</v>
       </c>
       <c r="C129">
@@ -6727,8 +6723,8 @@
       <c r="A130" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B130" s="10">
-        <f>AVERAGE(C130:N130)</f>
+      <c r="B130">
+        <f t="shared" ref="B130:B161" si="4">AVERAGE(C130:N130)</f>
         <v>25.833333333333332</v>
       </c>
       <c r="C130">
@@ -6772,8 +6768,8 @@
       <c r="A131" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B131" s="10">
-        <f>AVERAGE(C131:N131)</f>
+      <c r="B131">
+        <f t="shared" si="4"/>
         <v>23.416666666666668</v>
       </c>
       <c r="C131">
@@ -6817,8 +6813,8 @@
       <c r="A132" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B132" s="10">
-        <f>AVERAGE(C132:N132)</f>
+      <c r="B132">
+        <f t="shared" si="4"/>
         <v>1.0833333333333333</v>
       </c>
       <c r="C132">
@@ -6862,8 +6858,8 @@
       <c r="A133" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B133" s="10">
-        <f>AVERAGE(C133:N133)</f>
+      <c r="B133">
+        <f t="shared" si="4"/>
         <v>24.5</v>
       </c>
       <c r="C133">
@@ -6907,8 +6903,8 @@
       <c r="A134" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="B134" s="10">
-        <f>AVERAGE(C134:N134)</f>
+      <c r="B134">
+        <f t="shared" si="4"/>
         <v>84.583333333333329</v>
       </c>
       <c r="C134">
@@ -6956,26 +6952,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="18171fec-acf4-43d2-b526-0e7db5044e74">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="fcf87922-c7f3-44a4-9aa8-f585f70d1698" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F3EBF122F3DB854AB6515567219CA9AB" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="95866c8e7206fe2ad6c1db40d1ce538a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="18171fec-acf4-43d2-b526-0e7db5044e74" xmlns:ns3="fcf87922-c7f3-44a4-9aa8-f585f70d1698" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b9244ac4e6d70d4305f413f251a8df0d" ns2:_="" ns3:_="">
     <xsd:import namespace="18171fec-acf4-43d2-b526-0e7db5044e74"/>
@@ -7224,26 +7200,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE8CA7C7-0543-45CC-984E-159C73A18247}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="18171fec-acf4-43d2-b526-0e7db5044e74"/>
-    <ds:schemaRef ds:uri="fcf87922-c7f3-44a4-9aa8-f585f70d1698"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BE144DA-0517-4B44-8E1F-BCA276D302D0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="18171fec-acf4-43d2-b526-0e7db5044e74">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="fcf87922-c7f3-44a4-9aa8-f585f70d1698" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E9FB786-E036-4CB0-BC07-622D42DA0456}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7260,4 +7237,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BE144DA-0517-4B44-8E1F-BCA276D302D0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE8CA7C7-0543-45CC-984E-159C73A18247}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="18171fec-acf4-43d2-b526-0e7db5044e74"/>
+    <ds:schemaRef ds:uri="fcf87922-c7f3-44a4-9aa8-f585f70d1698"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>